<commit_message>
modified for non to theoretical 4 papers
</commit_message>
<xml_diff>
--- a/Overall Files/Analysis.xlsx
+++ b/Overall Files/Analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minsik/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minsik/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C9735835-1521-AE4A-8901-90BD460D9642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63DF5203-2160-E642-94E7-AED4816D6321}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{D191EDB1-F553-D84A-B803-B27A1F8FBA75}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19460" xr2:uid="{D191EDB1-F553-D84A-B803-B27A1F8FBA75}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1522" uniqueCount="553">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1518" uniqueCount="553">
   <si>
     <t>Title</t>
   </si>
@@ -1701,18 +1701,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1721,6 +1721,13 @@
       <color theme="1"/>
       <name val="Helvetica"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1745,11 +1752,11 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1765,7 +1772,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2063,16 +2070,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F78730E6-1DB0-FD44-93CC-339688788B9E}">
   <dimension ref="A1:K200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G175" workbookViewId="0">
-      <selection activeCell="K200" sqref="A1:K200"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="11" width="33.83203125" customWidth="1"/>
+    <col min="1" max="11" width="33.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2107,7 +2112,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -2136,7 +2141,7 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
@@ -2165,7 +2170,7 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
@@ -2194,7 +2199,7 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11">
       <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
@@ -2225,7 +2230,7 @@
       </c>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11">
       <c r="A6" s="1" t="s">
         <v>29</v>
       </c>
@@ -2256,7 +2261,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11">
       <c r="A7" s="1" t="s">
         <v>36</v>
       </c>
@@ -2285,7 +2290,7 @@
       </c>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11">
       <c r="A8" s="1" t="s">
         <v>41</v>
       </c>
@@ -2316,7 +2321,7 @@
       </c>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11">
       <c r="A9" s="1" t="s">
         <v>46</v>
       </c>
@@ -2347,7 +2352,7 @@
       </c>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11">
       <c r="A10" s="1" t="s">
         <v>49</v>
       </c>
@@ -2378,7 +2383,7 @@
       </c>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11">
       <c r="A11" s="1" t="s">
         <v>54</v>
       </c>
@@ -2409,7 +2414,7 @@
       </c>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11">
       <c r="A12" s="1" t="s">
         <v>57</v>
       </c>
@@ -2440,7 +2445,7 @@
       </c>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11">
       <c r="A13" s="1" t="s">
         <v>62</v>
       </c>
@@ -2471,7 +2476,7 @@
       </c>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11">
       <c r="A14" s="1" t="s">
         <v>65</v>
       </c>
@@ -2502,7 +2507,7 @@
       </c>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11">
       <c r="A15" s="1" t="s">
         <v>67</v>
       </c>
@@ -2524,16 +2529,14 @@
       <c r="G15" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>71</v>
-      </c>
+      <c r="H15" s="1"/>
       <c r="I15" s="2"/>
       <c r="J15" s="1" t="s">
         <v>28</v>
       </c>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11">
       <c r="A16" s="1" t="s">
         <v>72</v>
       </c>
@@ -2564,7 +2567,7 @@
       </c>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11">
       <c r="A17" s="1" t="s">
         <v>76</v>
       </c>
@@ -2595,7 +2598,7 @@
       </c>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11">
       <c r="A18" s="1" t="s">
         <v>79</v>
       </c>
@@ -2624,7 +2627,7 @@
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11">
       <c r="A19" s="1" t="s">
         <v>82</v>
       </c>
@@ -2653,7 +2656,7 @@
       </c>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11">
       <c r="A20" s="1" t="s">
         <v>84</v>
       </c>
@@ -2682,7 +2685,7 @@
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11">
       <c r="A21" s="1" t="s">
         <v>87</v>
       </c>
@@ -2713,7 +2716,7 @@
       </c>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11">
       <c r="A22" s="1" t="s">
         <v>90</v>
       </c>
@@ -2744,7 +2747,7 @@
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11">
       <c r="A23" s="1" t="s">
         <v>94</v>
       </c>
@@ -2775,7 +2778,7 @@
       </c>
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11">
       <c r="A24" s="1" t="s">
         <v>97</v>
       </c>
@@ -2806,7 +2809,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11">
       <c r="A25" s="1" t="s">
         <v>99</v>
       </c>
@@ -2835,7 +2838,7 @@
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11">
       <c r="A26" s="1" t="s">
         <v>103</v>
       </c>
@@ -2866,7 +2869,7 @@
       </c>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11">
       <c r="A27" s="1" t="s">
         <v>105</v>
       </c>
@@ -2897,7 +2900,7 @@
       </c>
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11">
       <c r="A28" s="1" t="s">
         <v>109</v>
       </c>
@@ -2928,7 +2931,7 @@
       </c>
       <c r="K28" s="2"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11">
       <c r="A29" s="1" t="s">
         <v>111</v>
       </c>
@@ -2957,7 +2960,7 @@
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11">
       <c r="A30" s="1" t="s">
         <v>114</v>
       </c>
@@ -2988,7 +2991,7 @@
       </c>
       <c r="K30" s="2"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11">
       <c r="A31" s="1" t="s">
         <v>116</v>
       </c>
@@ -3021,7 +3024,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11">
       <c r="A32" s="1" t="s">
         <v>118</v>
       </c>
@@ -3052,7 +3055,7 @@
       </c>
       <c r="K32" s="2"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11">
       <c r="A33" s="1" t="s">
         <v>121</v>
       </c>
@@ -3083,7 +3086,7 @@
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11">
       <c r="A34" s="1" t="s">
         <v>125</v>
       </c>
@@ -3110,7 +3113,7 @@
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11">
       <c r="A35" s="1" t="s">
         <v>128</v>
       </c>
@@ -3132,16 +3135,14 @@
       <c r="G35" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="H35" s="1" t="s">
-        <v>71</v>
-      </c>
+      <c r="H35" s="1"/>
       <c r="I35" s="2"/>
       <c r="J35" s="1" t="s">
         <v>28</v>
       </c>
       <c r="K35" s="2"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11">
       <c r="A36" s="1" t="s">
         <v>132</v>
       </c>
@@ -3172,7 +3173,7 @@
       </c>
       <c r="K36" s="2"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11">
       <c r="A37" s="1" t="s">
         <v>135</v>
       </c>
@@ -3203,7 +3204,7 @@
       </c>
       <c r="K37" s="2"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11">
       <c r="A38" s="1" t="s">
         <v>138</v>
       </c>
@@ -3236,7 +3237,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11">
       <c r="A39" s="1" t="s">
         <v>142</v>
       </c>
@@ -3269,7 +3270,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11">
       <c r="A40" s="1" t="s">
         <v>145</v>
       </c>
@@ -3300,7 +3301,7 @@
       </c>
       <c r="K40" s="2"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11">
       <c r="A41" s="1" t="s">
         <v>148</v>
       </c>
@@ -3327,7 +3328,7 @@
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11">
       <c r="A42" s="1" t="s">
         <v>152</v>
       </c>
@@ -3354,7 +3355,7 @@
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11">
       <c r="A43" s="1" t="s">
         <v>155</v>
       </c>
@@ -3383,7 +3384,7 @@
       </c>
       <c r="K43" s="2"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11">
       <c r="A44" s="1" t="s">
         <v>157</v>
       </c>
@@ -3414,7 +3415,7 @@
       </c>
       <c r="K44" s="2"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11">
       <c r="A45" s="1" t="s">
         <v>159</v>
       </c>
@@ -3445,7 +3446,7 @@
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11">
       <c r="A46" s="1" t="s">
         <v>161</v>
       </c>
@@ -3476,7 +3477,7 @@
       </c>
       <c r="K46" s="2"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11">
       <c r="A47" s="1" t="s">
         <v>165</v>
       </c>
@@ -3507,7 +3508,7 @@
       </c>
       <c r="K47" s="2"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11">
       <c r="A48" s="1" t="s">
         <v>169</v>
       </c>
@@ -3538,7 +3539,7 @@
       </c>
       <c r="K48" s="2"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11">
       <c r="A49" s="1" t="s">
         <v>172</v>
       </c>
@@ -3571,7 +3572,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11">
       <c r="A50" s="1" t="s">
         <v>175</v>
       </c>
@@ -3602,7 +3603,7 @@
       </c>
       <c r="K50" s="2"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11">
       <c r="A51" s="1" t="s">
         <v>179</v>
       </c>
@@ -3633,7 +3634,7 @@
       </c>
       <c r="K51" s="2"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11">
       <c r="A52" s="1" t="s">
         <v>183</v>
       </c>
@@ -3664,7 +3665,7 @@
       </c>
       <c r="K52" s="2"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11">
       <c r="A53" s="1" t="s">
         <v>186</v>
       </c>
@@ -3686,16 +3687,14 @@
       <c r="G53" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="H53" s="1" t="s">
-        <v>71</v>
-      </c>
+      <c r="H53" s="1"/>
       <c r="I53" s="2"/>
       <c r="J53" s="1" t="s">
         <v>28</v>
       </c>
       <c r="K53" s="2"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11">
       <c r="A54" s="1" t="s">
         <v>189</v>
       </c>
@@ -3726,7 +3725,7 @@
       </c>
       <c r="K54" s="2"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11">
       <c r="A55" s="1" t="s">
         <v>193</v>
       </c>
@@ -3757,7 +3756,7 @@
       </c>
       <c r="K55" s="2"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11">
       <c r="A56" s="1" t="s">
         <v>197</v>
       </c>
@@ -3788,7 +3787,7 @@
       </c>
       <c r="K56" s="2"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11">
       <c r="A57" s="1" t="s">
         <v>199</v>
       </c>
@@ -3817,7 +3816,7 @@
       <c r="J57" s="2"/>
       <c r="K57" s="2"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11">
       <c r="A58" s="1" t="s">
         <v>202</v>
       </c>
@@ -3846,7 +3845,7 @@
       <c r="J58" s="2"/>
       <c r="K58" s="2"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11">
       <c r="A59" s="1" t="s">
         <v>204</v>
       </c>
@@ -3873,7 +3872,7 @@
       <c r="J59" s="2"/>
       <c r="K59" s="2"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11">
       <c r="A60" s="1" t="s">
         <v>207</v>
       </c>
@@ -3904,7 +3903,7 @@
       <c r="J60" s="2"/>
       <c r="K60" s="2"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11">
       <c r="A61" s="1" t="s">
         <v>210</v>
       </c>
@@ -3935,7 +3934,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11">
       <c r="A62" s="1" t="s">
         <v>214</v>
       </c>
@@ -3966,7 +3965,7 @@
       </c>
       <c r="K62" s="2"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11">
       <c r="A63" s="1" t="s">
         <v>217</v>
       </c>
@@ -3997,7 +3996,7 @@
       </c>
       <c r="K63" s="2"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11">
       <c r="A64" s="1" t="s">
         <v>221</v>
       </c>
@@ -4030,7 +4029,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11">
       <c r="A65" s="1" t="s">
         <v>224</v>
       </c>
@@ -4061,7 +4060,7 @@
       </c>
       <c r="K65" s="2"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11">
       <c r="A66" s="1" t="s">
         <v>226</v>
       </c>
@@ -4092,7 +4091,7 @@
       </c>
       <c r="K66" s="2"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11">
       <c r="A67" s="1" t="s">
         <v>229</v>
       </c>
@@ -4125,7 +4124,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11">
       <c r="A68" s="1" t="s">
         <v>232</v>
       </c>
@@ -4154,7 +4153,7 @@
       <c r="J68" s="2"/>
       <c r="K68" s="2"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11">
       <c r="A69" s="1" t="s">
         <v>236</v>
       </c>
@@ -4185,7 +4184,7 @@
       </c>
       <c r="K69" s="2"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11">
       <c r="A70" s="1" t="s">
         <v>240</v>
       </c>
@@ -4216,7 +4215,7 @@
       </c>
       <c r="K70" s="2"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11">
       <c r="A71" s="1" t="s">
         <v>244</v>
       </c>
@@ -4245,7 +4244,7 @@
       <c r="J71" s="2"/>
       <c r="K71" s="2"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11">
       <c r="A72" s="1" t="s">
         <v>247</v>
       </c>
@@ -4276,7 +4275,7 @@
       </c>
       <c r="K72" s="2"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11">
       <c r="A73" s="1" t="s">
         <v>250</v>
       </c>
@@ -4307,7 +4306,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11">
       <c r="A74" s="1" t="s">
         <v>252</v>
       </c>
@@ -4334,7 +4333,7 @@
       <c r="J74" s="2"/>
       <c r="K74" s="2"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11">
       <c r="A75" s="1" t="s">
         <v>256</v>
       </c>
@@ -4365,7 +4364,7 @@
       </c>
       <c r="K75" s="2"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11">
       <c r="A76" s="1" t="s">
         <v>258</v>
       </c>
@@ -4394,7 +4393,7 @@
       </c>
       <c r="K76" s="2"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11">
       <c r="A77" s="1" t="s">
         <v>261</v>
       </c>
@@ -4425,7 +4424,7 @@
       </c>
       <c r="K77" s="2"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11">
       <c r="A78" s="1" t="s">
         <v>264</v>
       </c>
@@ -4458,7 +4457,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11">
       <c r="A79" s="1" t="s">
         <v>267</v>
       </c>
@@ -4487,7 +4486,7 @@
       </c>
       <c r="K79" s="2"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11">
       <c r="A80" s="1" t="s">
         <v>270</v>
       </c>
@@ -4518,7 +4517,7 @@
       </c>
       <c r="K80" s="2"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:11">
       <c r="A81" s="1" t="s">
         <v>273</v>
       </c>
@@ -4547,7 +4546,7 @@
       </c>
       <c r="K81" s="2"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:11">
       <c r="A82" s="1" t="s">
         <v>275</v>
       </c>
@@ -4576,7 +4575,7 @@
       <c r="J82" s="2"/>
       <c r="K82" s="2"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11">
       <c r="A83" s="1" t="s">
         <v>277</v>
       </c>
@@ -4605,7 +4604,7 @@
       </c>
       <c r="K83" s="2"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11">
       <c r="A84" s="1" t="s">
         <v>279</v>
       </c>
@@ -4636,7 +4635,7 @@
       </c>
       <c r="K84" s="2"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11">
       <c r="A85" s="1" t="s">
         <v>282</v>
       </c>
@@ -4667,7 +4666,7 @@
       </c>
       <c r="K85" s="2"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11">
       <c r="A86" s="1" t="s">
         <v>286</v>
       </c>
@@ -4696,7 +4695,7 @@
       </c>
       <c r="K86" s="2"/>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:11">
       <c r="A87" s="1" t="s">
         <v>289</v>
       </c>
@@ -4729,7 +4728,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:11">
       <c r="A88" s="1" t="s">
         <v>292</v>
       </c>
@@ -4760,7 +4759,7 @@
       </c>
       <c r="K88" s="2"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:11">
       <c r="A89" s="1" t="s">
         <v>295</v>
       </c>
@@ -4787,7 +4786,7 @@
       <c r="J89" s="2"/>
       <c r="K89" s="2"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:11">
       <c r="A90" s="1" t="s">
         <v>299</v>
       </c>
@@ -4818,7 +4817,7 @@
       </c>
       <c r="K90" s="2"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:11">
       <c r="A91" s="1" t="s">
         <v>302</v>
       </c>
@@ -4847,7 +4846,7 @@
       </c>
       <c r="K91" s="2"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:11">
       <c r="A92" s="1" t="s">
         <v>305</v>
       </c>
@@ -4878,7 +4877,7 @@
       </c>
       <c r="K92" s="2"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:11">
       <c r="A93" s="1" t="s">
         <v>307</v>
       </c>
@@ -4909,7 +4908,7 @@
       </c>
       <c r="K93" s="2"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:11">
       <c r="A94" s="1" t="s">
         <v>309</v>
       </c>
@@ -4936,7 +4935,7 @@
       <c r="J94" s="2"/>
       <c r="K94" s="2"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:11">
       <c r="A95" s="1" t="s">
         <v>311</v>
       </c>
@@ -4967,7 +4966,7 @@
       </c>
       <c r="K95" s="2"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:11">
       <c r="A96" s="1" t="s">
         <v>313</v>
       </c>
@@ -4996,7 +4995,7 @@
       </c>
       <c r="K96" s="2"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:11">
       <c r="A97" s="1" t="s">
         <v>315</v>
       </c>
@@ -5023,7 +5022,7 @@
       <c r="J97" s="2"/>
       <c r="K97" s="2"/>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:11">
       <c r="A98" s="1" t="s">
         <v>317</v>
       </c>
@@ -5050,7 +5049,7 @@
       <c r="J98" s="2"/>
       <c r="K98" s="2"/>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:11">
       <c r="A99" s="1" t="s">
         <v>321</v>
       </c>
@@ -5079,7 +5078,7 @@
       <c r="J99" s="2"/>
       <c r="K99" s="2"/>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:11">
       <c r="A100" s="1" t="s">
         <v>325</v>
       </c>
@@ -5110,7 +5109,7 @@
       <c r="J100" s="2"/>
       <c r="K100" s="2"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:11">
       <c r="A101" s="1" t="s">
         <v>329</v>
       </c>
@@ -5139,7 +5138,7 @@
       <c r="J101" s="2"/>
       <c r="K101" s="2"/>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:11">
       <c r="A102" s="1" t="s">
         <v>333</v>
       </c>
@@ -5170,7 +5169,7 @@
       </c>
       <c r="K102" s="2"/>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:11">
       <c r="A103" s="1" t="s">
         <v>337</v>
       </c>
@@ -5201,7 +5200,7 @@
       </c>
       <c r="K103" s="2"/>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:11">
       <c r="A104" s="1" t="s">
         <v>341</v>
       </c>
@@ -5232,7 +5231,7 @@
       </c>
       <c r="K104" s="2"/>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:11">
       <c r="A105" s="1" t="s">
         <v>344</v>
       </c>
@@ -5261,7 +5260,7 @@
       </c>
       <c r="K105" s="2"/>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:11">
       <c r="A106" s="1" t="s">
         <v>346</v>
       </c>
@@ -5292,7 +5291,7 @@
       </c>
       <c r="K106" s="2"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:11">
       <c r="A107" s="1" t="s">
         <v>349</v>
       </c>
@@ -5321,7 +5320,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:11">
       <c r="A108" s="1" t="s">
         <v>352</v>
       </c>
@@ -5352,7 +5351,7 @@
       </c>
       <c r="K108" s="2"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:11">
       <c r="A109" s="1" t="s">
         <v>355</v>
       </c>
@@ -5385,7 +5384,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:11">
       <c r="A110" s="1" t="s">
         <v>358</v>
       </c>
@@ -5416,7 +5415,7 @@
       </c>
       <c r="K110" s="2"/>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:11">
       <c r="A111" s="1" t="s">
         <v>363</v>
       </c>
@@ -5449,7 +5448,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:11">
       <c r="A112" s="1" t="s">
         <v>365</v>
       </c>
@@ -5480,7 +5479,7 @@
       </c>
       <c r="K112" s="2"/>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:11">
       <c r="A113" s="1" t="s">
         <v>367</v>
       </c>
@@ -5507,7 +5506,7 @@
       <c r="J113" s="2"/>
       <c r="K113" s="2"/>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:11">
       <c r="A114" s="1" t="s">
         <v>370</v>
       </c>
@@ -5538,7 +5537,7 @@
       </c>
       <c r="K114" s="2"/>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:11">
       <c r="A115" s="1" t="s">
         <v>372</v>
       </c>
@@ -5569,7 +5568,7 @@
       </c>
       <c r="K115" s="2"/>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:11">
       <c r="A116" s="1" t="s">
         <v>374</v>
       </c>
@@ -5596,7 +5595,7 @@
       <c r="J116" s="2"/>
       <c r="K116" s="2"/>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:11">
       <c r="A117" s="1" t="s">
         <v>378</v>
       </c>
@@ -5627,7 +5626,7 @@
       </c>
       <c r="K117" s="2"/>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:11">
       <c r="A118" s="1" t="s">
         <v>381</v>
       </c>
@@ -5654,7 +5653,7 @@
       <c r="J118" s="2"/>
       <c r="K118" s="2"/>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:11">
       <c r="A119" s="1" t="s">
         <v>383</v>
       </c>
@@ -5681,7 +5680,7 @@
       <c r="J119" s="2"/>
       <c r="K119" s="2"/>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:11">
       <c r="A120" s="1" t="s">
         <v>385</v>
       </c>
@@ -5712,7 +5711,7 @@
       </c>
       <c r="K120" s="2"/>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:11">
       <c r="A121" s="1" t="s">
         <v>388</v>
       </c>
@@ -5741,7 +5740,7 @@
       <c r="J121" s="2"/>
       <c r="K121" s="2"/>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:11">
       <c r="A122" s="1" t="s">
         <v>390</v>
       </c>
@@ -5772,7 +5771,7 @@
       </c>
       <c r="K122" s="2"/>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:11">
       <c r="A123" s="1" t="s">
         <v>393</v>
       </c>
@@ -5801,7 +5800,7 @@
       <c r="J123" s="2"/>
       <c r="K123" s="2"/>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:11">
       <c r="A124" s="1" t="s">
         <v>395</v>
       </c>
@@ -5830,7 +5829,7 @@
       </c>
       <c r="K124" s="2"/>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:11">
       <c r="A125" s="1" t="s">
         <v>397</v>
       </c>
@@ -5861,7 +5860,7 @@
       </c>
       <c r="K125" s="2"/>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:11">
       <c r="A126" s="1" t="s">
         <v>400</v>
       </c>
@@ -5890,7 +5889,7 @@
       <c r="J126" s="2"/>
       <c r="K126" s="2"/>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:11">
       <c r="A127" s="1" t="s">
         <v>402</v>
       </c>
@@ -5921,7 +5920,7 @@
       </c>
       <c r="K127" s="2"/>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:11">
       <c r="A128" s="1" t="s">
         <v>404</v>
       </c>
@@ -5948,7 +5947,7 @@
       <c r="J128" s="2"/>
       <c r="K128" s="2"/>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:11">
       <c r="A129" s="1" t="s">
         <v>406</v>
       </c>
@@ -5977,7 +5976,7 @@
       </c>
       <c r="K129" s="2"/>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:11">
       <c r="A130" s="1" t="s">
         <v>408</v>
       </c>
@@ -6006,7 +6005,7 @@
       <c r="J130" s="2"/>
       <c r="K130" s="2"/>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:11">
       <c r="A131" s="1" t="s">
         <v>410</v>
       </c>
@@ -6037,7 +6036,7 @@
       </c>
       <c r="K131" s="2"/>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:11">
       <c r="A132" s="1" t="s">
         <v>412</v>
       </c>
@@ -6066,7 +6065,7 @@
       <c r="J132" s="2"/>
       <c r="K132" s="2"/>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:11">
       <c r="A133" s="1" t="s">
         <v>414</v>
       </c>
@@ -6095,7 +6094,7 @@
       <c r="J133" s="2"/>
       <c r="K133" s="2"/>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:11">
       <c r="A134" s="1" t="s">
         <v>417</v>
       </c>
@@ -6124,7 +6123,7 @@
       <c r="J134" s="2"/>
       <c r="K134" s="2"/>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:11">
       <c r="A135" s="1" t="s">
         <v>419</v>
       </c>
@@ -6155,7 +6154,7 @@
       </c>
       <c r="K135" s="2"/>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:11">
       <c r="A136" s="1" t="s">
         <v>421</v>
       </c>
@@ -6186,7 +6185,7 @@
       </c>
       <c r="K136" s="2"/>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:11">
       <c r="A137" s="1" t="s">
         <v>423</v>
       </c>
@@ -6215,7 +6214,7 @@
       <c r="J137" s="2"/>
       <c r="K137" s="2"/>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:11">
       <c r="A138" s="1" t="s">
         <v>425</v>
       </c>
@@ -6246,7 +6245,7 @@
       </c>
       <c r="K138" s="2"/>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:11">
       <c r="A139" s="1" t="s">
         <v>426</v>
       </c>
@@ -6277,7 +6276,7 @@
       </c>
       <c r="K139" s="2"/>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:11">
       <c r="A140" s="1" t="s">
         <v>428</v>
       </c>
@@ -6308,7 +6307,7 @@
       </c>
       <c r="K140" s="2"/>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:11">
       <c r="A141" s="1" t="s">
         <v>430</v>
       </c>
@@ -6339,7 +6338,7 @@
       </c>
       <c r="K141" s="2"/>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:11">
       <c r="A142" s="1" t="s">
         <v>432</v>
       </c>
@@ -6368,7 +6367,7 @@
       <c r="J142" s="2"/>
       <c r="K142" s="2"/>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:11">
       <c r="A143" s="1" t="s">
         <v>433</v>
       </c>
@@ -6395,7 +6394,7 @@
       <c r="J143" s="2"/>
       <c r="K143" s="2"/>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:11">
       <c r="A144" s="1" t="s">
         <v>435</v>
       </c>
@@ -6426,7 +6425,7 @@
       </c>
       <c r="K144" s="2"/>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:11">
       <c r="A145" s="1" t="s">
         <v>437</v>
       </c>
@@ -6457,7 +6456,7 @@
       </c>
       <c r="K145" s="2"/>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:11">
       <c r="A146" s="1" t="s">
         <v>439</v>
       </c>
@@ -6486,7 +6485,7 @@
       <c r="J146" s="2"/>
       <c r="K146" s="2"/>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:11">
       <c r="A147" s="1" t="s">
         <v>441</v>
       </c>
@@ -6515,7 +6514,7 @@
       <c r="J147" s="2"/>
       <c r="K147" s="2"/>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:11">
       <c r="A148" s="1" t="s">
         <v>443</v>
       </c>
@@ -6544,7 +6543,7 @@
       </c>
       <c r="K148" s="2"/>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:11">
       <c r="A149" s="1" t="s">
         <v>445</v>
       </c>
@@ -6573,7 +6572,7 @@
       <c r="J149" s="2"/>
       <c r="K149" s="2"/>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:11">
       <c r="A150" s="1" t="s">
         <v>447</v>
       </c>
@@ -6600,7 +6599,7 @@
       <c r="J150" s="2"/>
       <c r="K150" s="2"/>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:11">
       <c r="A151" s="1" t="s">
         <v>449</v>
       </c>
@@ -6629,7 +6628,7 @@
       <c r="J151" s="2"/>
       <c r="K151" s="2"/>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:11">
       <c r="A152" s="1" t="s">
         <v>451</v>
       </c>
@@ -6660,7 +6659,7 @@
       </c>
       <c r="K152" s="2"/>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:11">
       <c r="A153" s="1" t="s">
         <v>453</v>
       </c>
@@ -6689,7 +6688,7 @@
       <c r="J153" s="2"/>
       <c r="K153" s="2"/>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:11">
       <c r="A154" s="1" t="s">
         <v>456</v>
       </c>
@@ -6720,7 +6719,7 @@
       <c r="J154" s="2"/>
       <c r="K154" s="2"/>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:11">
       <c r="A155" s="1" t="s">
         <v>458</v>
       </c>
@@ -6753,7 +6752,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:11">
       <c r="A156" s="1" t="s">
         <v>460</v>
       </c>
@@ -6784,7 +6783,7 @@
       </c>
       <c r="K156" s="2"/>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:11">
       <c r="A157" s="1" t="s">
         <v>462</v>
       </c>
@@ -6811,7 +6810,7 @@
       <c r="J157" s="2"/>
       <c r="K157" s="2"/>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:11">
       <c r="A158" s="1" t="s">
         <v>464</v>
       </c>
@@ -6840,7 +6839,7 @@
       </c>
       <c r="K158" s="2"/>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:11">
       <c r="A159" s="1" t="s">
         <v>466</v>
       </c>
@@ -6871,7 +6870,7 @@
       </c>
       <c r="K159" s="2"/>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:11">
       <c r="A160" s="1" t="s">
         <v>468</v>
       </c>
@@ -6900,7 +6899,7 @@
       <c r="J160" s="2"/>
       <c r="K160" s="2"/>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:11">
       <c r="A161" s="1" t="s">
         <v>470</v>
       </c>
@@ -6929,7 +6928,7 @@
       <c r="J161" s="2"/>
       <c r="K161" s="2"/>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:11">
       <c r="A162" s="1" t="s">
         <v>472</v>
       </c>
@@ -6960,7 +6959,7 @@
       </c>
       <c r="K162" s="2"/>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:11">
       <c r="A163" s="1" t="s">
         <v>474</v>
       </c>
@@ -6989,7 +6988,7 @@
       <c r="J163" s="2"/>
       <c r="K163" s="2"/>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:11">
       <c r="A164" s="1" t="s">
         <v>476</v>
       </c>
@@ -7022,7 +7021,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:11">
       <c r="A165" s="1" t="s">
         <v>478</v>
       </c>
@@ -7053,7 +7052,7 @@
       </c>
       <c r="K165" s="2"/>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:11">
       <c r="A166" s="1" t="s">
         <v>480</v>
       </c>
@@ -7082,7 +7081,7 @@
       </c>
       <c r="K166" s="2"/>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:11">
       <c r="A167" s="1" t="s">
         <v>482</v>
       </c>
@@ -7113,7 +7112,7 @@
       </c>
       <c r="K167" s="2"/>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:11">
       <c r="A168" s="1" t="s">
         <v>484</v>
       </c>
@@ -7146,7 +7145,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:11">
       <c r="A169" s="1" t="s">
         <v>486</v>
       </c>
@@ -7177,7 +7176,7 @@
       </c>
       <c r="K169" s="2"/>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:11">
       <c r="A170" s="1" t="s">
         <v>488</v>
       </c>
@@ -7208,7 +7207,7 @@
       </c>
       <c r="K170" s="2"/>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:11">
       <c r="A171" s="1" t="s">
         <v>490</v>
       </c>
@@ -7239,7 +7238,7 @@
       </c>
       <c r="K171" s="2"/>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:11">
       <c r="A172" s="1" t="s">
         <v>491</v>
       </c>
@@ -7268,7 +7267,7 @@
       <c r="J172" s="2"/>
       <c r="K172" s="2"/>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:11">
       <c r="A173" s="1" t="s">
         <v>494</v>
       </c>
@@ -7297,7 +7296,7 @@
       <c r="J173" s="2"/>
       <c r="K173" s="2"/>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:11">
       <c r="A174" s="1" t="s">
         <v>497</v>
       </c>
@@ -7326,7 +7325,7 @@
       <c r="J174" s="2"/>
       <c r="K174" s="2"/>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:11">
       <c r="A175" s="1" t="s">
         <v>499</v>
       </c>
@@ -7357,7 +7356,7 @@
       </c>
       <c r="K175" s="2"/>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:11">
       <c r="A176" s="1" t="s">
         <v>501</v>
       </c>
@@ -7388,7 +7387,7 @@
       </c>
       <c r="K176" s="2"/>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:11">
       <c r="A177" s="1" t="s">
         <v>503</v>
       </c>
@@ -7419,7 +7418,7 @@
       </c>
       <c r="K177" s="2"/>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:11">
       <c r="A178" s="1" t="s">
         <v>505</v>
       </c>
@@ -7446,7 +7445,7 @@
       <c r="J178" s="2"/>
       <c r="K178" s="2"/>
     </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:11">
       <c r="A179" s="1" t="s">
         <v>507</v>
       </c>
@@ -7475,7 +7474,7 @@
       </c>
       <c r="K179" s="2"/>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:11">
       <c r="A180" s="1" t="s">
         <v>509</v>
       </c>
@@ -7504,7 +7503,7 @@
       </c>
       <c r="K180" s="2"/>
     </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:11">
       <c r="A181" s="1" t="s">
         <v>511</v>
       </c>
@@ -7531,7 +7530,7 @@
       <c r="J181" s="2"/>
       <c r="K181" s="2"/>
     </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:11">
       <c r="A182" s="1" t="s">
         <v>513</v>
       </c>
@@ -7562,7 +7561,7 @@
       </c>
       <c r="K182" s="2"/>
     </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:11">
       <c r="A183" s="1" t="s">
         <v>515</v>
       </c>
@@ -7591,7 +7590,7 @@
       </c>
       <c r="K183" s="2"/>
     </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:11">
       <c r="A184" s="1" t="s">
         <v>517</v>
       </c>
@@ -7624,7 +7623,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:11">
       <c r="A185" s="1" t="s">
         <v>519</v>
       </c>
@@ -7657,7 +7656,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:11">
       <c r="A186" s="1" t="s">
         <v>522</v>
       </c>
@@ -7686,7 +7685,7 @@
       <c r="J186" s="2"/>
       <c r="K186" s="2"/>
     </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:11">
       <c r="A187" s="1" t="s">
         <v>524</v>
       </c>
@@ -7713,7 +7712,7 @@
       <c r="J187" s="2"/>
       <c r="K187" s="2"/>
     </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:11">
       <c r="A188" s="1" t="s">
         <v>526</v>
       </c>
@@ -7742,7 +7741,7 @@
       <c r="J188" s="2"/>
       <c r="K188" s="2"/>
     </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:11">
       <c r="A189" s="1" t="s">
         <v>528</v>
       </c>
@@ -7773,7 +7772,7 @@
       </c>
       <c r="K189" s="2"/>
     </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:11">
       <c r="A190" s="1" t="s">
         <v>530</v>
       </c>
@@ -7804,7 +7803,7 @@
       </c>
       <c r="K190" s="2"/>
     </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:11">
       <c r="A191" s="1" t="s">
         <v>533</v>
       </c>
@@ -7826,16 +7825,14 @@
       <c r="G191" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="H191" s="1" t="s">
-        <v>71</v>
-      </c>
+      <c r="H191" s="1"/>
       <c r="I191" s="1" t="s">
         <v>34</v>
       </c>
       <c r="J191" s="2"/>
       <c r="K191" s="2"/>
     </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:11">
       <c r="A192" s="1" t="s">
         <v>535</v>
       </c>
@@ -7866,7 +7863,7 @@
       </c>
       <c r="K192" s="2"/>
     </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:11">
       <c r="A193" s="1" t="s">
         <v>537</v>
       </c>
@@ -7897,7 +7894,7 @@
       </c>
       <c r="K193" s="2"/>
     </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:11">
       <c r="A194" s="1" t="s">
         <v>539</v>
       </c>
@@ -7928,7 +7925,7 @@
       </c>
       <c r="K194" s="2"/>
     </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:11">
       <c r="A195" s="1" t="s">
         <v>541</v>
       </c>
@@ -7961,7 +7958,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:11">
       <c r="A196" s="1" t="s">
         <v>542</v>
       </c>
@@ -7992,7 +7989,7 @@
       </c>
       <c r="K196" s="2"/>
     </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:11">
       <c r="A197" s="1" t="s">
         <v>544</v>
       </c>
@@ -8021,7 +8018,7 @@
       <c r="J197" s="2"/>
       <c r="K197" s="2"/>
     </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:11">
       <c r="A198" s="1" t="s">
         <v>546</v>
       </c>
@@ -8052,7 +8049,7 @@
       </c>
       <c r="K198" s="2"/>
     </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:11">
       <c r="A199" s="1" t="s">
         <v>548</v>
       </c>
@@ -8083,7 +8080,7 @@
       </c>
       <c r="K199" s="2"/>
     </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:11">
       <c r="A200" s="1" t="s">
         <v>549</v>
       </c>
@@ -8115,6 +8112,7 @@
       <c r="K200" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>